<commit_message>
timesheet update for carol
</commit_message>
<xml_diff>
--- a/admin/Timesheets/Caroline Chang/Week 3 Timesheet.xlsx
+++ b/admin/Timesheets/Caroline Chang/Week 3 Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\CSCI_Classes\CSCI4308\capstone_proj\admin\Timesheets\Caroline Chang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54383C9E-08F0-4685-9FF1-F03F6B301DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF1E571-FE6B-4949-96D3-35FD97ABB278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="1956" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Mentor Meeting</t>
+  </si>
+  <si>
+    <t>Charter Work</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:K11"/>
+  <dimension ref="A4:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,20 +517,33 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>1.5</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1">
+      <c r="C12" s="1">
         <v>0.5</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1">
+      <c r="D12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>